<commit_message>
Malzeme List SQL App - Some fixes
</commit_message>
<xml_diff>
--- a/malzeme_list_sql_app/assets/database/malzeme_backup.xlsx
+++ b/malzeme_list_sql_app/assets/database/malzeme_backup.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
   <si>
     <t xml:space="preserve">Malzeme</t>
   </si>
@@ -23,172 +23,271 @@
     <t xml:space="preserve">Açıklama</t>
   </si>
   <si>
+    <t xml:space="preserve">Adaptör (USB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Adaptör (USB) (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ampul (beyaz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ampul LED (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayakkabı çekeceği (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banyo kesesi (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bel çantası (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bornoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crocs terlik (sokak)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk 5 TB (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolap stoperi (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don (erkek)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dürbün (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eldiven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eldiven (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elektrikli el tornavidası (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethernet Kablo (UTP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eğe (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Güç korumalı priz</t>
+  </si>
+  <si>
     <t xml:space="preserve">HDMI Kablo</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethernet Kablo (UTP)</t>
+    <t xml:space="preserve">Havlu (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Havlu (banyo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iki port USB adaptör (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapı altı stoper (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapı stoperi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapı stoperi (Silikon)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karga burun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kasket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaşar (migros)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koli bandı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontrol kalemi (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krema (migros)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kulaklık (kablolu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kızartma Tenceresi (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED lamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Led fener yuvarlak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lif (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maket bıçağı (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masa lastiği (ayak)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masa örtü kıskacı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merdane (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mini USB kablo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modem tel kablosu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oklava (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pense (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perde kancası</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perde stoperi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pijama (erkek)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pijama (kadın)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pil (Kalın)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pil (İnce)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeater (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeater (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensörlü (LED) (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensörlü Lamba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinek ilacı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinek ilacı sprey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinek raketi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinek İlacı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sıvı yağ (migros)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-Shirt (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-shirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabure (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahta kaşık (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahta çubuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teflon tava (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tencere (Ufak) (Eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tornavida (Düz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tornavida (Yıldız)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tornavida seti (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toz bezi (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB - Ethernet çevirici (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB 3.0 kablo (Ankara)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB Kablo (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB hub ethernetli (eksik)</t>
   </si>
   <si>
     <t xml:space="preserve">Uzatma kablosu</t>
   </si>
   <si>
-    <t xml:space="preserve">Adaptör (USB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Güç korumalı priz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koli bandı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Post it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pil (Kalın)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pil (İnce)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensörlü Lamba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eldiven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Led fener yuvarlak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masa örtü kıskacı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tornavida (Yıldız)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tornavida (Düz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karga burun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapı stoperi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masa lastiği (ayak)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahta çubuk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perde stoperi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perde kancası</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapı stoperi (Silikon)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metre</t>
+    <t xml:space="preserve">Uzatma kablosu - USB (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wifi repater (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yan keski (eksik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoğurt kasesi (eksik)</t>
   </si>
   <si>
     <t xml:space="preserve">Çekiç (eksik)</t>
   </si>
   <si>
-    <t xml:space="preserve">Kontrol kalemi (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maket bıçağı (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yan keski (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pense (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tornavida seti (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elektrikli el tornavidası (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adaptör (USB) (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB Kablo (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ampul (beyaz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ampul LED (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bornoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dolap stoperi (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eldiven (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-shirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinek ilacı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lif (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banyo kesesi (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dürbün (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eğe (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ayakkabı çekeceği (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinek ilacı sprey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wifi repater (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB hub ethernetli (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabure (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oklava (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensörlü (LED) (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeater (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yoğurt kasesi (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahta kaşık (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modem tel kablosu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toz bezi (eksik)</t>
+    <t xml:space="preserve">Çorap (kısa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Çorap (orta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Çorap (uzun)</t>
   </si>
   <si>
     <t xml:space="preserve">Çöp tenekesi (eksik)</t>
@@ -197,115 +296,7 @@
     <t xml:space="preserve">Şapka</t>
   </si>
   <si>
-    <t xml:space="preserve">Kasket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mayo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapı altı stoper (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaşar (migros)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sıvı yağ (migros)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krema (migros)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mini USB kablo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uzatma kablosu - USB (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pijama (erkek)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pijama (kadın)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Havlu (banyo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinek raketi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinek İlacı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iki port USB adaptör (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB - Ethernet çevirici (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeater (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eski tel (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disk 5 TB (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB 3.0 kablo (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kızartma Tenceresi (eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED lamba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bel çantası (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tencere (Ufak) (Eksik)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teflon tava (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Havlu (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merdane (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T-Shirt (Ankara)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Şort (Ankara)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kulaklık (kablolu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crocs terlik (sokak)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don (erkek)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Çorap (kısa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erkek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Çorap (orta)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">erkek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Çorap (uzun)</t>
   </si>
 </sst>
 </file>
@@ -591,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -602,7 +593,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -613,7 +604,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -624,7 +615,7 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -635,7 +626,7 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -668,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -679,7 +670,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -690,7 +681,7 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -701,7 +692,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -712,7 +703,7 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -734,7 +725,7 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -745,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -767,7 +758,7 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -778,7 +769,7 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -789,7 +780,7 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -800,7 +791,7 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -811,7 +802,7 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -844,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -855,7 +846,7 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -866,7 +857,7 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -877,7 +868,7 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -899,7 +890,7 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -907,10 +898,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -918,7 +909,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -929,10 +920,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -940,10 +931,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -951,10 +942,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -962,7 +953,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -973,7 +964,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -984,7 +975,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -995,10 +986,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1006,10 +997,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -1017,10 +1008,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -1028,10 +1019,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>4</v>
@@ -1039,10 +1030,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
@@ -1050,10 +1041,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -1061,10 +1052,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -1072,10 +1063,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -1083,7 +1074,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1094,10 +1085,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -1105,10 +1096,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -1116,10 +1107,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -1127,10 +1118,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
@@ -1138,10 +1129,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
         <v>4</v>
@@ -1149,10 +1140,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
@@ -1163,7 +1154,7 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
         <v>4</v>
@@ -1174,7 +1165,7 @@
         <v>57</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -1185,7 +1176,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
         <v>4</v>
@@ -1207,7 +1198,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C59" t="s">
         <v>4</v>
@@ -1218,7 +1209,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
         <v>4</v>
@@ -1240,7 +1231,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -1251,7 +1242,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
         <v>4</v>
@@ -1262,7 +1253,7 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
@@ -1284,7 +1275,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
@@ -1295,7 +1286,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
         <v>4</v>
@@ -1306,7 +1297,7 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
@@ -1317,7 +1308,7 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -1328,7 +1319,7 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70" t="s">
         <v>4</v>
@@ -1339,7 +1330,7 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
         <v>4</v>
@@ -1361,7 +1352,7 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s">
         <v>4</v>
@@ -1394,7 +1385,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" t="s">
         <v>4</v>
@@ -1405,7 +1396,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
@@ -1427,7 +1418,7 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
         <v>4</v>
@@ -1438,7 +1429,7 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" t="s">
         <v>4</v>
@@ -1449,7 +1440,7 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
         <v>4</v>
@@ -1482,7 +1473,7 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
@@ -1504,7 +1495,7 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -1515,7 +1506,7 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
         <v>4</v>
@@ -1526,7 +1517,7 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C88" t="s">
         <v>4</v>
@@ -1559,7 +1550,7 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C91" t="s">
         <v>4</v>
@@ -1570,32 +1561,21 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>97</v>
-      </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-      <c r="C94" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>